<commit_message>
delete .empty and complete framework test
</commit_message>
<xml_diff>
--- a/feasibility-analysis/feasibility-analysis.xlsx
+++ b/feasibility-analysis/feasibility-analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin Ssu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Graduation-Project\feasibility-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4364FE-EA76-4E13-8C0E-B948041A9933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F812A9-2837-4FFE-8B0F-0DF385CA6C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C524DE1E-122D-431B-9986-3C54448ABE0B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>挑戰</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,34 @@
   </si>
   <si>
     <t>實際結果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試 react + sprint boot + mongo db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斯培哲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用 API 戶相連接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>能夠正常執行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>React 的 package.json 要加上聽後端 8080 port 那段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -110,9 +138,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B475F2AA-3FCA-4F58-9686-F51A56C544F1}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -479,6 +510,38 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45571</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45571</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>